<commit_message>
dto ok , form add/up/details , todo assignement
</commit_message>
<xml_diff>
--- a/doc/backlog.xlsx
+++ b/doc/backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\come_\Desktop\formation_spring\wacdo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF312E7-CB5F-4659-A12E-1BD7482EA060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E21885-DF91-42B8-A02C-3A7759B6A806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="13546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>operation</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>1 day</t>
-  </si>
-  <si>
-    <t>1 dat</t>
   </si>
   <si>
     <t>security implementation</t>
@@ -286,6 +283,15 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -293,15 +299,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -587,7 +584,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -598,172 +595,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" ht="37.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>